<commit_message>
SRS version 1.5 , signal modes added
</commit_message>
<xml_diff>
--- a/SWE/Software Specification/SRS/SRS review.xlsx
+++ b/SWE/Software Specification/SRS/SRS review.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Sovy - Digital Calculator PO1_DGC</t>
   </si>
@@ -88,6 +88,21 @@
   </si>
   <si>
     <t>Requirements 3,4,5,6,11,12</t>
+  </si>
+  <si>
+    <t>Specify operation signal and its modes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Done</t>
+  </si>
+  <si>
+    <t>Add table of mapping between signals and modes</t>
+  </si>
+  <si>
+    <t>Modify the requirements based on modes of signals</t>
+  </si>
+  <si>
+    <t>All Requirements</t>
   </si>
 </sst>
 </file>
@@ -449,13 +464,13 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="37.88671875" customWidth="1"/>
-    <col min="4" max="4" width="32.88671875" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" customWidth="1"/>
+    <col min="4" max="4" width="45.21875" customWidth="1"/>
     <col min="9" max="9" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -705,10 +720,18 @@
     <row r="8" spans="1:26" ht="13.2">
       <c r="A8" s="1"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="16">
+        <v>44300</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
       <c r="I8" s="10"/>
@@ -733,10 +756,18 @@
     <row r="9" spans="1:26" ht="13.2">
       <c r="A9" s="1"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="10"/>
+      <c r="C9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="16">
+        <v>44301</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
       <c r="I9" s="10"/>

</xml_diff>

<commit_message>
GDD + RTM done
</commit_message>
<xml_diff>
--- a/SWE/Software Specification/SRS/SRS review.xlsx
+++ b/SWE/Software Specification/SRS/SRS review.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Sovy - Digital Calculator PO1_DGC</t>
   </si>
@@ -88,6 +88,21 @@
   </si>
   <si>
     <t>Requirements 3,4,5,6,11,12</t>
+  </si>
+  <si>
+    <t>Specify operation signal and its modes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Done</t>
+  </si>
+  <si>
+    <t>Add table of mapping between signals and modes</t>
+  </si>
+  <si>
+    <t>Modify the requirements based on modes of signals</t>
+  </si>
+  <si>
+    <t>All Requirements</t>
   </si>
 </sst>
 </file>
@@ -449,13 +464,13 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="37.88671875" customWidth="1"/>
-    <col min="4" max="4" width="32.88671875" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" customWidth="1"/>
+    <col min="4" max="4" width="45.21875" customWidth="1"/>
     <col min="9" max="9" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -705,10 +720,18 @@
     <row r="8" spans="1:26" ht="13.2">
       <c r="A8" s="1"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="16">
+        <v>44300</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
       <c r="I8" s="10"/>
@@ -733,10 +756,18 @@
     <row r="9" spans="1:26" ht="13.2">
       <c r="A9" s="1"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="10"/>
+      <c r="C9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="16">
+        <v>44301</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
       <c r="I9" s="10"/>

</xml_diff>